<commit_message>
autoAttack rework, Skills wip
</commit_message>
<xml_diff>
--- a/Documents/Todo - Prototype.xlsx
+++ b/Documents/Todo - Prototype.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Documents\ESGI\Projet Annuel\Alterego\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB45723-A20F-470F-BE0E-9E07BFD4184D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>ToDo liste</t>
   </si>
@@ -52,9 +61,6 @@
     <t>Selon l'idée Labo :
 peu de grande salles
 multitudes de petites salles reliées</t>
-  </si>
-  <si>
-    <t>Création d'un terrain de test pour le Prototype qui sera à revoir pour la suite des jalons</t>
   </si>
   <si>
     <t>sauvegarder sa progression (de son avancée dans le jeu, de son avatar ou du
@@ -107,137 +113,176 @@
   <si>
     <t>boutique de skins du joueur, monnais recupéré a chaque run</t>
   </si>
+  <si>
+    <t xml:space="preserve">génération de niveau aléatoire
+</t>
+  </si>
+  <si>
+    <t>reimplémentation de l'environnement avec une generation aléatoire</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="8">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -427,252 +472,247 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="24.71"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="8" t="s">
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" ht="39.75" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" ht="49.5" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="1" t="s">
+    <row r="14" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" ht="51.75" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" ht="48.75" customHeight="1">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="10"/>
+      <c r="C15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="11" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" ht="51.75" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="8" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="10"/>
+      <c r="E17" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" ht="45.75" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" ht="66.75" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" ht="84.0" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" ht="75.0" customHeight="1">
-      <c r="A21" s="8" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" ht="149.25" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="149.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A11:B12"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
     <mergeCell ref="A21:B22"/>
     <mergeCell ref="C21:D22"/>
     <mergeCell ref="E21:E22"/>
@@ -683,7 +723,30 @@
     <mergeCell ref="C15:D16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="C5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="A5:B6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>